<commit_message>
Rerun DLinear on new dataset
</commit_message>
<xml_diff>
--- a/Model/DLinear/processing_output/CMG/622/close_test_scaler.xlsx
+++ b/Model/DLinear/processing_output/CMG/622/close_test_scaler.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B251"/>
+  <dimension ref="A1:B263"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,7 +445,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.81003</v>
+        <v>0.64837</v>
       </c>
     </row>
     <row r="3">
@@ -453,7 +453,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.82162</v>
+        <v>0.62908</v>
       </c>
     </row>
     <row r="4">
@@ -461,7 +461,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.77319</v>
+        <v>0.62778</v>
       </c>
     </row>
     <row r="5">
@@ -469,7 +469,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.80218</v>
+        <v>0.58693</v>
       </c>
     </row>
     <row r="6">
@@ -477,7 +477,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.8837</v>
+        <v>0.52157</v>
       </c>
     </row>
     <row r="7">
@@ -485,7 +485,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.85266</v>
+        <v>0.46275</v>
       </c>
     </row>
     <row r="8">
@@ -493,7 +493,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0.8605</v>
+        <v>0.49346</v>
       </c>
     </row>
     <row r="9">
@@ -501,7 +501,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.8779</v>
+        <v>0.54967</v>
       </c>
     </row>
     <row r="10">
@@ -509,7 +509,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0.96351</v>
+        <v>0.51275</v>
       </c>
     </row>
     <row r="11">
@@ -517,7 +517,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0.98738</v>
+        <v>0.53954</v>
       </c>
     </row>
     <row r="12">
@@ -525,7 +525,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>0.97954</v>
+        <v>0.53954</v>
       </c>
     </row>
     <row r="13">
@@ -533,7 +533,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>1.04366</v>
+        <v>0.4768</v>
       </c>
     </row>
     <row r="14">
@@ -541,7 +541,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>1.0382</v>
+        <v>0.53431</v>
       </c>
     </row>
     <row r="15">
@@ -549,7 +549,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>1.00341</v>
+        <v>0.56013</v>
       </c>
     </row>
     <row r="16">
@@ -557,7 +557,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>1.01671</v>
+        <v>0.55882</v>
       </c>
     </row>
     <row r="17">
@@ -565,7 +565,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>0.98738</v>
+        <v>0.55752</v>
       </c>
     </row>
     <row r="18">
@@ -573,7 +573,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>0.98738</v>
+        <v>0.56373</v>
       </c>
     </row>
     <row r="19">
@@ -581,7 +581,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>0.97954</v>
+        <v>0.54967</v>
       </c>
     </row>
     <row r="20">
@@ -589,7 +589,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>0.89666</v>
+        <v>0.57026</v>
       </c>
     </row>
     <row r="21">
@@ -597,7 +597,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>0.92087</v>
+        <v>0.58039</v>
       </c>
     </row>
     <row r="22">
@@ -605,7 +605,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>0.86733</v>
+        <v>0.61111</v>
       </c>
     </row>
     <row r="23">
@@ -613,7 +613,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>0.81924</v>
+        <v>0.6545800000000001</v>
       </c>
     </row>
     <row r="24">
@@ -621,7 +621,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>0.8512999999999999</v>
+        <v>0.69804</v>
       </c>
     </row>
     <row r="25">
@@ -629,7 +629,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>0.76603</v>
+        <v>0.69314</v>
       </c>
     </row>
     <row r="26">
@@ -637,7 +637,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>0.78854</v>
+        <v>0.71863</v>
       </c>
     </row>
     <row r="27">
@@ -645,7 +645,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>0.81651</v>
+        <v>0.69804</v>
       </c>
     </row>
     <row r="28">
@@ -653,7 +653,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>0.76739</v>
+        <v>0.66732</v>
       </c>
     </row>
     <row r="29">
@@ -661,7 +661,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>0.6886100000000001</v>
+        <v>0.65588</v>
       </c>
     </row>
     <row r="30">
@@ -669,7 +669,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>0.73666</v>
+        <v>0.68791</v>
       </c>
     </row>
     <row r="31">
@@ -677,7 +677,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>0.65928</v>
+        <v>0.66732</v>
       </c>
     </row>
     <row r="32">
@@ -685,7 +685,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>0.71248</v>
+        <v>0.67778</v>
       </c>
     </row>
     <row r="33">
@@ -693,7 +693,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>0.74727</v>
+        <v>0.6686299999999999</v>
       </c>
     </row>
     <row r="34">
@@ -701,7 +701,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>0.7073700000000001</v>
+        <v>0.6598000000000001</v>
       </c>
     </row>
     <row r="35">
@@ -709,7 +709,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>0.69645</v>
+        <v>0.66242</v>
       </c>
     </row>
     <row r="36">
@@ -717,7 +717,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>0.70464</v>
+        <v>0.6571900000000001</v>
       </c>
     </row>
     <row r="37">
@@ -725,7 +725,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>0.72063</v>
+        <v>0.6571900000000001</v>
       </c>
     </row>
     <row r="38">
@@ -733,7 +733,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>0.72063</v>
+        <v>0.62647</v>
       </c>
     </row>
     <row r="39">
@@ -741,7 +741,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>0.70464</v>
+        <v>0.61765</v>
       </c>
     </row>
     <row r="40">
@@ -749,7 +749,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>0.64325</v>
+        <v>0.64314</v>
       </c>
     </row>
     <row r="41">
@@ -757,7 +757,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>0.6698499999999999</v>
+        <v>0.64183</v>
       </c>
     </row>
     <row r="42">
@@ -765,7 +765,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>0.68042</v>
+        <v>0.58824</v>
       </c>
     </row>
     <row r="43">
@@ -773,7 +773,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>0.68997</v>
+        <v>0.62124</v>
       </c>
     </row>
     <row r="44">
@@ -781,7 +781,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>0.68588</v>
+        <v>0.61634</v>
       </c>
     </row>
     <row r="45">
@@ -789,7 +789,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>0.67667</v>
+        <v>0.63922</v>
       </c>
     </row>
     <row r="46">
@@ -797,7 +797,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>0.65655</v>
+        <v>0.66732</v>
       </c>
     </row>
     <row r="47">
@@ -805,7 +805,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>0.65518</v>
+        <v>0.70585</v>
       </c>
     </row>
     <row r="48">
@@ -813,7 +813,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>0.61255</v>
+        <v>0.69539</v>
       </c>
     </row>
     <row r="49">
@@ -821,7 +821,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>0.54434</v>
+        <v>0.69804</v>
       </c>
     </row>
     <row r="50">
@@ -829,7 +829,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>0.48295</v>
+        <v>0.6918</v>
       </c>
     </row>
     <row r="51">
@@ -837,7 +837,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>0.51501</v>
+        <v>0.66732</v>
       </c>
     </row>
     <row r="52">
@@ -845,7 +845,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>0.57367</v>
+        <v>0.70327</v>
       </c>
     </row>
     <row r="53">
@@ -853,7 +853,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>0.53513</v>
+        <v>0.6892200000000001</v>
       </c>
     </row>
     <row r="54">
@@ -861,7 +861,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>0.5631</v>
+        <v>0.68007</v>
       </c>
     </row>
     <row r="55">
@@ -869,7 +869,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>0.5631</v>
+        <v>0.67386</v>
       </c>
     </row>
     <row r="56">
@@ -877,7 +877,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>0.49761</v>
+        <v>0.67516</v>
       </c>
     </row>
     <row r="57">
@@ -885,7 +885,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>0.55764</v>
+        <v>0.68007</v>
       </c>
     </row>
     <row r="58">
@@ -893,7 +893,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>0.58458</v>
+        <v>0.69314</v>
       </c>
     </row>
     <row r="59">
@@ -901,7 +901,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>0.58322</v>
+        <v>0.70814</v>
       </c>
     </row>
     <row r="60">
@@ -909,7 +909,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>0.58186</v>
+        <v>0.75686</v>
       </c>
     </row>
     <row r="61">
@@ -917,7 +917,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>0.58834</v>
+        <v>0.74412</v>
       </c>
     </row>
     <row r="62">
@@ -925,7 +925,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>0.57367</v>
+        <v>0.74673</v>
       </c>
     </row>
     <row r="63">
@@ -933,7 +933,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>0.59516</v>
+        <v>0.70814</v>
       </c>
     </row>
     <row r="64">
@@ -941,7 +941,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>0.60573</v>
+        <v>0.72876</v>
       </c>
     </row>
     <row r="65">
@@ -949,7 +949,7 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>0.63779</v>
+        <v>0.74412</v>
       </c>
     </row>
     <row r="66">
@@ -957,7 +957,7 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>0.68315</v>
+        <v>0.73137</v>
       </c>
     </row>
     <row r="67">
@@ -965,7 +965,7 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>0.72851</v>
+        <v>0.70065</v>
       </c>
     </row>
     <row r="68">
@@ -973,7 +973,7 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>0.7234</v>
+        <v>0.71732</v>
       </c>
     </row>
     <row r="69">
@@ -981,7 +981,7 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>0.75</v>
+        <v>0.71732</v>
       </c>
     </row>
     <row r="70">
@@ -989,7 +989,7 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>0.72851</v>
+        <v>0.70585</v>
       </c>
     </row>
     <row r="71">
@@ -997,7 +997,7 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>0.69645</v>
+        <v>0.71601</v>
       </c>
     </row>
     <row r="72">
@@ -1005,7 +1005,7 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>0.68452</v>
+        <v>0.71601</v>
       </c>
     </row>
     <row r="73">
@@ -1013,7 +1013,7 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>0.71794</v>
+        <v>0.70814</v>
       </c>
     </row>
     <row r="74">
@@ -1021,7 +1021,7 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>0.69645</v>
+        <v>0.70065</v>
       </c>
     </row>
     <row r="75">
@@ -1029,7 +1029,7 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>0.7073700000000001</v>
+        <v>0.69935</v>
       </c>
     </row>
     <row r="76">
@@ -1037,7 +1037,7 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>0.69782</v>
+        <v>0.71601</v>
       </c>
     </row>
     <row r="77">
@@ -1045,7 +1045,7 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>0.6886100000000001</v>
+        <v>0.71601</v>
       </c>
     </row>
     <row r="78">
@@ -1053,7 +1053,7 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>0.69134</v>
+        <v>0.66732</v>
       </c>
     </row>
     <row r="79">
@@ -1061,7 +1061,7 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>0.68588</v>
+        <v>0.69049</v>
       </c>
     </row>
     <row r="80">
@@ -1069,7 +1069,7 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>0.68588</v>
+        <v>0.68137</v>
       </c>
     </row>
     <row r="81">
@@ -1077,7 +1077,7 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>0.65382</v>
+        <v>0.66471</v>
       </c>
     </row>
     <row r="82">
@@ -1085,7 +1085,7 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>0.64461</v>
+        <v>0.68268</v>
       </c>
     </row>
     <row r="83">
@@ -1093,7 +1093,7 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>0.67121</v>
+        <v>0.69049</v>
       </c>
     </row>
     <row r="84">
@@ -1101,7 +1101,7 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>0.6698499999999999</v>
+        <v>0.67876</v>
       </c>
     </row>
     <row r="85">
@@ -1109,7 +1109,7 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>0.61392</v>
+        <v>0.64935</v>
       </c>
     </row>
     <row r="86">
@@ -1117,7 +1117,7 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>0.64836</v>
+        <v>0.67876</v>
       </c>
     </row>
     <row r="87">
@@ -1125,7 +1125,7 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>0.64325</v>
+        <v>0.67647</v>
       </c>
     </row>
     <row r="88">
@@ -1133,7 +1133,7 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>0.66712</v>
+        <v>0.68529</v>
       </c>
     </row>
     <row r="89">
@@ -1141,7 +1141,7 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>0.69645</v>
+        <v>0.68007</v>
       </c>
     </row>
     <row r="90">
@@ -1149,7 +1149,7 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>0.73666</v>
+        <v>0.69314</v>
       </c>
     </row>
     <row r="91">
@@ -1157,7 +1157,7 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>0.72575</v>
+        <v>0.68791</v>
       </c>
     </row>
     <row r="92">
@@ -1165,7 +1165,7 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>0.72851</v>
+        <v>0.65196</v>
       </c>
     </row>
     <row r="93">
@@ -1173,7 +1173,7 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>0.722</v>
+        <v>0.70065</v>
       </c>
     </row>
     <row r="94">
@@ -1181,7 +1181,7 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>0.69645</v>
+        <v>0.69314</v>
       </c>
     </row>
     <row r="95">
@@ -1189,7 +1189,7 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>0.73397</v>
+        <v>0.69539</v>
       </c>
     </row>
     <row r="96">
@@ -1197,7 +1197,7 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>0.7193000000000001</v>
+        <v>0.67516</v>
       </c>
     </row>
     <row r="97">
@@ -1205,7 +1205,7 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>0.70975</v>
+        <v>0.6918</v>
       </c>
     </row>
     <row r="98">
@@ -1213,7 +1213,7 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>0.70327</v>
+        <v>0.6918</v>
       </c>
     </row>
     <row r="99">
@@ -1221,7 +1221,7 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>0.70464</v>
+        <v>0.6585</v>
       </c>
     </row>
     <row r="100">
@@ -1229,7 +1229,7 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>0.70975</v>
+        <v>0.68399</v>
       </c>
     </row>
     <row r="101">
@@ -1237,7 +1237,7 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>0.7234</v>
+        <v>0.6598000000000001</v>
       </c>
     </row>
     <row r="102">
@@ -1245,7 +1245,7 @@
         <v>100</v>
       </c>
       <c r="B102" t="n">
-        <v>0.73905</v>
+        <v>0.66471</v>
       </c>
     </row>
     <row r="103">
@@ -1253,7 +1253,7 @@
         <v>101</v>
       </c>
       <c r="B103" t="n">
-        <v>0.7899</v>
+        <v>0.66242</v>
       </c>
     </row>
     <row r="104">
@@ -1261,7 +1261,7 @@
         <v>102</v>
       </c>
       <c r="B104" t="n">
-        <v>0.7766</v>
+        <v>0.6571900000000001</v>
       </c>
     </row>
     <row r="105">
@@ -1269,7 +1269,7 @@
         <v>103</v>
       </c>
       <c r="B105" t="n">
-        <v>0.77933</v>
+        <v>0.67255</v>
       </c>
     </row>
     <row r="106">
@@ -1277,7 +1277,7 @@
         <v>104</v>
       </c>
       <c r="B106" t="n">
-        <v>0.73905</v>
+        <v>0.66732</v>
       </c>
     </row>
     <row r="107">
@@ -1285,7 +1285,7 @@
         <v>105</v>
       </c>
       <c r="B107" t="n">
-        <v>0.76057</v>
+        <v>0.6598000000000001</v>
       </c>
     </row>
     <row r="108">
@@ -1293,7 +1293,7 @@
         <v>106</v>
       </c>
       <c r="B108" t="n">
-        <v>0.7766</v>
+        <v>0.69314</v>
       </c>
     </row>
     <row r="109">
@@ -1301,7 +1301,7 @@
         <v>107</v>
       </c>
       <c r="B109" t="n">
-        <v>0.7633</v>
+        <v>0.71863</v>
       </c>
     </row>
     <row r="110">
@@ -1309,7 +1309,7 @@
         <v>108</v>
       </c>
       <c r="B110" t="n">
-        <v>0.73124</v>
+        <v>0.71078</v>
       </c>
     </row>
     <row r="111">
@@ -1317,7 +1317,7 @@
         <v>109</v>
       </c>
       <c r="B111" t="n">
-        <v>0.74864</v>
+        <v>0.70585</v>
       </c>
     </row>
     <row r="112">
@@ -1325,7 +1325,7 @@
         <v>110</v>
       </c>
       <c r="B112" t="n">
-        <v>0.74864</v>
+        <v>0.71078</v>
       </c>
     </row>
     <row r="113">
@@ -1333,7 +1333,7 @@
         <v>111</v>
       </c>
       <c r="B113" t="n">
-        <v>0.73666</v>
+        <v>0.7134</v>
       </c>
     </row>
     <row r="114">
@@ -1341,7 +1341,7 @@
         <v>112</v>
       </c>
       <c r="B114" t="n">
-        <v>0.74727</v>
+        <v>0.70719</v>
       </c>
     </row>
     <row r="115">
@@ -1349,7 +1349,7 @@
         <v>113</v>
       </c>
       <c r="B115" t="n">
-        <v>0.74727</v>
+        <v>0.70065</v>
       </c>
     </row>
     <row r="116">
@@ -1357,7 +1357,7 @@
         <v>114</v>
       </c>
       <c r="B116" t="n">
-        <v>0.73905</v>
+        <v>0.69804</v>
       </c>
     </row>
     <row r="117">
@@ -1365,7 +1365,7 @@
         <v>115</v>
       </c>
       <c r="B117" t="n">
-        <v>0.73124</v>
+        <v>0.70327</v>
       </c>
     </row>
     <row r="118">
@@ -1373,7 +1373,7 @@
         <v>116</v>
       </c>
       <c r="B118" t="n">
-        <v>0.72988</v>
+        <v>0.69804</v>
       </c>
     </row>
     <row r="119">
@@ -1381,7 +1381,7 @@
         <v>117</v>
       </c>
       <c r="B119" t="n">
-        <v>0.74727</v>
+        <v>0.69935</v>
       </c>
     </row>
     <row r="120">
@@ -1389,7 +1389,7 @@
         <v>118</v>
       </c>
       <c r="B120" t="n">
-        <v>0.74727</v>
+        <v>0.71601</v>
       </c>
     </row>
     <row r="121">
@@ -1397,7 +1397,7 @@
         <v>119</v>
       </c>
       <c r="B121" t="n">
-        <v>0.69645</v>
+        <v>0.69804</v>
       </c>
     </row>
     <row r="122">
@@ -1405,7 +1405,7 @@
         <v>120</v>
       </c>
       <c r="B122" t="n">
-        <v>0.72063</v>
+        <v>0.68529</v>
       </c>
     </row>
     <row r="123">
@@ -1413,7 +1413,7 @@
         <v>121</v>
       </c>
       <c r="B123" t="n">
-        <v>0.71112</v>
+        <v>0.69539</v>
       </c>
     </row>
     <row r="124">
@@ -1421,7 +1421,7 @@
         <v>122</v>
       </c>
       <c r="B124" t="n">
-        <v>0.69372</v>
+        <v>0.69314</v>
       </c>
     </row>
     <row r="125">
@@ -1429,7 +1429,7 @@
         <v>123</v>
       </c>
       <c r="B125" t="n">
-        <v>0.71248</v>
+        <v>0.69539</v>
       </c>
     </row>
     <row r="126">
@@ -1437,7 +1437,7 @@
         <v>124</v>
       </c>
       <c r="B126" t="n">
-        <v>0.72063</v>
+        <v>0.69935</v>
       </c>
     </row>
     <row r="127">
@@ -1445,7 +1445,7 @@
         <v>125</v>
       </c>
       <c r="B127" t="n">
-        <v>0.70839</v>
+        <v>0.69673</v>
       </c>
     </row>
     <row r="128">
@@ -1453,7 +1453,7 @@
         <v>126</v>
       </c>
       <c r="B128" t="n">
-        <v>0.67769</v>
+        <v>0.6918</v>
       </c>
     </row>
     <row r="129">
@@ -1461,7 +1461,7 @@
         <v>127</v>
       </c>
       <c r="B129" t="n">
-        <v>0.70839</v>
+        <v>0.69314</v>
       </c>
     </row>
     <row r="130">
@@ -1469,7 +1469,7 @@
         <v>128</v>
       </c>
       <c r="B130" t="n">
-        <v>0.706</v>
+        <v>0.69314</v>
       </c>
     </row>
     <row r="131">
@@ -1477,7 +1477,7 @@
         <v>129</v>
       </c>
       <c r="B131" t="n">
-        <v>0.71521</v>
+        <v>0.7045400000000001</v>
       </c>
     </row>
     <row r="132">
@@ -1485,7 +1485,7 @@
         <v>130</v>
       </c>
       <c r="B132" t="n">
-        <v>0.70975</v>
+        <v>0.6892200000000001</v>
       </c>
     </row>
     <row r="133">
@@ -1493,7 +1493,7 @@
         <v>131</v>
       </c>
       <c r="B133" t="n">
-        <v>0.7234</v>
+        <v>0.68529</v>
       </c>
     </row>
     <row r="134">
@@ -1501,7 +1501,7 @@
         <v>132</v>
       </c>
       <c r="B134" t="n">
-        <v>0.71794</v>
+        <v>0.67386</v>
       </c>
     </row>
     <row r="135">
@@ -1509,7 +1509,7 @@
         <v>133</v>
       </c>
       <c r="B135" t="n">
-        <v>0.68042</v>
+        <v>0.69314</v>
       </c>
     </row>
     <row r="136">
@@ -1517,7 +1517,7 @@
         <v>134</v>
       </c>
       <c r="B136" t="n">
-        <v>0.73124</v>
+        <v>0.69935</v>
       </c>
     </row>
     <row r="137">
@@ -1525,7 +1525,7 @@
         <v>135</v>
       </c>
       <c r="B137" t="n">
-        <v>0.7234</v>
+        <v>0.68007</v>
       </c>
     </row>
     <row r="138">
@@ -1533,7 +1533,7 @@
         <v>136</v>
       </c>
       <c r="B138" t="n">
-        <v>0.72575</v>
+        <v>0.67647</v>
       </c>
     </row>
     <row r="139">
@@ -1541,7 +1541,7 @@
         <v>137</v>
       </c>
       <c r="B139" t="n">
-        <v>0.70464</v>
+        <v>0.67647</v>
       </c>
     </row>
     <row r="140">
@@ -1549,7 +1549,7 @@
         <v>138</v>
       </c>
       <c r="B140" t="n">
-        <v>0.722</v>
+        <v>0.6866</v>
       </c>
     </row>
     <row r="141">
@@ -1557,7 +1557,7 @@
         <v>139</v>
       </c>
       <c r="B141" t="n">
-        <v>0.722</v>
+        <v>0.68529</v>
       </c>
     </row>
     <row r="142">
@@ -1565,7 +1565,7 @@
         <v>140</v>
       </c>
       <c r="B142" t="n">
-        <v>0.68724</v>
+        <v>0.68007</v>
       </c>
     </row>
     <row r="143">
@@ -1573,7 +1573,7 @@
         <v>141</v>
       </c>
       <c r="B143" t="n">
-        <v>0.71385</v>
+        <v>0.69673</v>
       </c>
     </row>
     <row r="144">
@@ -1581,7 +1581,7 @@
         <v>142</v>
       </c>
       <c r="B144" t="n">
-        <v>0.6886100000000001</v>
+        <v>0.69314</v>
       </c>
     </row>
     <row r="145">
@@ -1589,7 +1589,7 @@
         <v>143</v>
       </c>
       <c r="B145" t="n">
-        <v>0.69372</v>
+        <v>0.6892200000000001</v>
       </c>
     </row>
     <row r="146">
@@ -1597,7 +1597,7 @@
         <v>144</v>
       </c>
       <c r="B146" t="n">
-        <v>0.69134</v>
+        <v>0.69314</v>
       </c>
     </row>
     <row r="147">
@@ -1605,7 +1605,7 @@
         <v>145</v>
       </c>
       <c r="B147" t="n">
-        <v>0.68588</v>
+        <v>0.69804</v>
       </c>
     </row>
     <row r="148">
@@ -1613,7 +1613,7 @@
         <v>146</v>
       </c>
       <c r="B148" t="n">
-        <v>0.70191</v>
+        <v>0.77092</v>
       </c>
     </row>
     <row r="149">
@@ -1621,7 +1621,7 @@
         <v>147</v>
       </c>
       <c r="B149" t="n">
-        <v>0.69645</v>
+        <v>0.81307</v>
       </c>
     </row>
     <row r="150">
@@ -1629,7 +1629,7 @@
         <v>148</v>
       </c>
       <c r="B150" t="n">
-        <v>0.6886100000000001</v>
+        <v>0.8081700000000001</v>
       </c>
     </row>
     <row r="151">
@@ -1637,7 +1637,7 @@
         <v>149</v>
       </c>
       <c r="B151" t="n">
-        <v>0.7234</v>
+        <v>0.78235</v>
       </c>
     </row>
     <row r="152">
@@ -1645,7 +1645,7 @@
         <v>150</v>
       </c>
       <c r="B152" t="n">
-        <v>0.75</v>
+        <v>0.8081700000000001</v>
       </c>
     </row>
     <row r="153">
@@ -1653,7 +1653,7 @@
         <v>151</v>
       </c>
       <c r="B153" t="n">
-        <v>0.74181</v>
+        <v>0.8081700000000001</v>
       </c>
     </row>
     <row r="154">
@@ -1661,7 +1661,7 @@
         <v>152</v>
       </c>
       <c r="B154" t="n">
-        <v>0.73666</v>
+        <v>0.79281</v>
       </c>
     </row>
     <row r="155">
@@ -1669,7 +1669,7 @@
         <v>153</v>
       </c>
       <c r="B155" t="n">
-        <v>0.74181</v>
+        <v>0.7902</v>
       </c>
     </row>
     <row r="156">
@@ -1677,7 +1677,7 @@
         <v>154</v>
       </c>
       <c r="B156" t="n">
-        <v>0.74454</v>
+        <v>0.79542</v>
       </c>
     </row>
     <row r="157">
@@ -1685,7 +1685,7 @@
         <v>155</v>
       </c>
       <c r="B157" t="n">
-        <v>0.73806</v>
+        <v>0.8081700000000001</v>
       </c>
     </row>
     <row r="158">
@@ -1693,7 +1693,7 @@
         <v>156</v>
       </c>
       <c r="B158" t="n">
-        <v>0.73124</v>
+        <v>0.80425</v>
       </c>
     </row>
     <row r="159">
@@ -1701,7 +1701,7 @@
         <v>157</v>
       </c>
       <c r="B159" t="n">
-        <v>0.72851</v>
+        <v>0.82092</v>
       </c>
     </row>
     <row r="160">
@@ -1709,7 +1709,7 @@
         <v>158</v>
       </c>
       <c r="B160" t="n">
-        <v>0.73397</v>
+        <v>0.81569</v>
       </c>
     </row>
     <row r="161">
@@ -1717,7 +1717,7 @@
         <v>159</v>
       </c>
       <c r="B161" t="n">
-        <v>0.72851</v>
+        <v>0.8081700000000001</v>
       </c>
     </row>
     <row r="162">
@@ -1725,7 +1725,7 @@
         <v>160</v>
       </c>
       <c r="B162" t="n">
-        <v>0.72988</v>
+        <v>0.80294</v>
       </c>
     </row>
     <row r="163">
@@ -1733,7 +1733,7 @@
         <v>161</v>
       </c>
       <c r="B163" t="n">
-        <v>0.74727</v>
+        <v>0.88105</v>
       </c>
     </row>
     <row r="164">
@@ -1741,7 +1741,7 @@
         <v>162</v>
       </c>
       <c r="B164" t="n">
-        <v>0.72851</v>
+        <v>0.86046</v>
       </c>
     </row>
     <row r="165">
@@ -1749,7 +1749,7 @@
         <v>163</v>
       </c>
       <c r="B165" t="n">
-        <v>0.71521</v>
+        <v>0.84641</v>
       </c>
     </row>
     <row r="166">
@@ -1757,7 +1757,7 @@
         <v>164</v>
       </c>
       <c r="B166" t="n">
-        <v>0.72575</v>
+        <v>0.83235</v>
       </c>
     </row>
     <row r="167">
@@ -1765,7 +1765,7 @@
         <v>165</v>
       </c>
       <c r="B167" t="n">
-        <v>0.7234</v>
+        <v>0.82582</v>
       </c>
     </row>
     <row r="168">
@@ -1773,7 +1773,7 @@
         <v>166</v>
       </c>
       <c r="B168" t="n">
-        <v>0.72575</v>
+        <v>0.83105</v>
       </c>
     </row>
     <row r="169">
@@ -1781,7 +1781,7 @@
         <v>167</v>
       </c>
       <c r="B169" t="n">
-        <v>0.72988</v>
+        <v>0.83889</v>
       </c>
     </row>
     <row r="170">
@@ -1789,7 +1789,7 @@
         <v>168</v>
       </c>
       <c r="B170" t="n">
-        <v>0.72715</v>
+        <v>0.8451</v>
       </c>
     </row>
     <row r="171">
@@ -1797,7 +1797,7 @@
         <v>169</v>
       </c>
       <c r="B171" t="n">
-        <v>0.722</v>
+        <v>0.84118</v>
       </c>
     </row>
     <row r="172">
@@ -1805,7 +1805,7 @@
         <v>170</v>
       </c>
       <c r="B172" t="n">
-        <v>0.7234</v>
+        <v>0.84379</v>
       </c>
     </row>
     <row r="173">
@@ -1813,7 +1813,7 @@
         <v>171</v>
       </c>
       <c r="B173" t="n">
-        <v>0.7234</v>
+        <v>0.84118</v>
       </c>
     </row>
     <row r="174">
@@ -1821,7 +1821,7 @@
         <v>172</v>
       </c>
       <c r="B174" t="n">
-        <v>0.7353</v>
+        <v>0.85294</v>
       </c>
     </row>
     <row r="175">
@@ -1829,7 +1829,7 @@
         <v>173</v>
       </c>
       <c r="B175" t="n">
-        <v>0.7193000000000001</v>
+        <v>0.86438</v>
       </c>
     </row>
     <row r="176">
@@ -1837,7 +1837,7 @@
         <v>174</v>
       </c>
       <c r="B176" t="n">
-        <v>0.71521</v>
+        <v>0.87582</v>
       </c>
     </row>
     <row r="177">
@@ -1845,7 +1845,7 @@
         <v>175</v>
       </c>
       <c r="B177" t="n">
-        <v>0.70327</v>
+        <v>0.8719</v>
       </c>
     </row>
     <row r="178">
@@ -1853,7 +1853,7 @@
         <v>176</v>
       </c>
       <c r="B178" t="n">
-        <v>0.7234</v>
+        <v>0.87712</v>
       </c>
     </row>
     <row r="179">
@@ -1861,7 +1861,7 @@
         <v>177</v>
       </c>
       <c r="B179" t="n">
-        <v>0.72988</v>
+        <v>0.88464</v>
       </c>
     </row>
     <row r="180">
@@ -1869,7 +1869,7 @@
         <v>178</v>
       </c>
       <c r="B180" t="n">
-        <v>0.70975</v>
+        <v>0.88366</v>
       </c>
     </row>
     <row r="181">
@@ -1877,7 +1877,7 @@
         <v>179</v>
       </c>
       <c r="B181" t="n">
-        <v>0.706</v>
+        <v>0.87451</v>
       </c>
     </row>
     <row r="182">
@@ -1885,7 +1885,7 @@
         <v>180</v>
       </c>
       <c r="B182" t="n">
-        <v>0.706</v>
+        <v>0.86961</v>
       </c>
     </row>
     <row r="183">
@@ -1893,7 +1893,7 @@
         <v>181</v>
       </c>
       <c r="B183" t="n">
-        <v>0.71658</v>
+        <v>0.8683</v>
       </c>
     </row>
     <row r="184">
@@ -1901,7 +1901,7 @@
         <v>182</v>
       </c>
       <c r="B184" t="n">
-        <v>0.71521</v>
+        <v>0.85654</v>
       </c>
     </row>
     <row r="185">
@@ -1909,7 +1909,7 @@
         <v>183</v>
       </c>
       <c r="B185" t="n">
-        <v>0.70975</v>
+        <v>0.85163</v>
       </c>
     </row>
     <row r="186">
@@ -1917,7 +1917,7 @@
         <v>184</v>
       </c>
       <c r="B186" t="n">
-        <v>0.72715</v>
+        <v>0.86699</v>
       </c>
     </row>
     <row r="187">
@@ -1925,7 +1925,7 @@
         <v>185</v>
       </c>
       <c r="B187" t="n">
-        <v>0.7234</v>
+        <v>0.87974</v>
       </c>
     </row>
     <row r="188">
@@ -1933,7 +1933,7 @@
         <v>186</v>
       </c>
       <c r="B188" t="n">
-        <v>0.7193000000000001</v>
+        <v>0.89902</v>
       </c>
     </row>
     <row r="189">
@@ -1941,7 +1941,7 @@
         <v>187</v>
       </c>
       <c r="B189" t="n">
-        <v>0.7234</v>
+        <v>0.89902</v>
       </c>
     </row>
     <row r="190">
@@ -1949,7 +1949,7 @@
         <v>188</v>
       </c>
       <c r="B190" t="n">
-        <v>0.72851</v>
+        <v>0.91046</v>
       </c>
     </row>
     <row r="191">
@@ -1957,7 +1957,7 @@
         <v>189</v>
       </c>
       <c r="B191" t="n">
-        <v>0.80457</v>
+        <v>0.89771</v>
       </c>
     </row>
     <row r="192">
@@ -1965,7 +1965,7 @@
         <v>190</v>
       </c>
       <c r="B192" t="n">
-        <v>0.84857</v>
+        <v>0.90261</v>
       </c>
     </row>
     <row r="193">
@@ -1973,7 +1973,7 @@
         <v>191</v>
       </c>
       <c r="B193" t="n">
-        <v>0.84345</v>
+        <v>0.90784</v>
       </c>
     </row>
     <row r="194">
@@ -1981,7 +1981,7 @@
         <v>192</v>
       </c>
       <c r="B194" t="n">
-        <v>0.81651</v>
+        <v>0.90261</v>
       </c>
     </row>
     <row r="195">
@@ -1989,7 +1989,7 @@
         <v>193</v>
       </c>
       <c r="B195" t="n">
-        <v>0.84345</v>
+        <v>0.89771</v>
       </c>
     </row>
     <row r="196">
@@ -1997,7 +1997,7 @@
         <v>194</v>
       </c>
       <c r="B196" t="n">
-        <v>0.84345</v>
+        <v>0.8951</v>
       </c>
     </row>
     <row r="197">
@@ -2005,7 +2005,7 @@
         <v>195</v>
       </c>
       <c r="B197" t="n">
-        <v>0.82742</v>
+        <v>0.89771</v>
       </c>
     </row>
     <row r="198">
@@ -2013,7 +2013,7 @@
         <v>196</v>
       </c>
       <c r="B198" t="n">
-        <v>0.82469</v>
+        <v>0.8924800000000001</v>
       </c>
     </row>
     <row r="199">
@@ -2021,7 +2021,7 @@
         <v>197</v>
       </c>
       <c r="B199" t="n">
-        <v>0.8301500000000001</v>
+        <v>0.89641</v>
       </c>
     </row>
     <row r="200">
@@ -2029,7 +2029,7 @@
         <v>198</v>
       </c>
       <c r="B200" t="n">
-        <v>0.84345</v>
+        <v>0.89902</v>
       </c>
     </row>
     <row r="201">
@@ -2037,7 +2037,7 @@
         <v>199</v>
       </c>
       <c r="B201" t="n">
-        <v>0.83936</v>
+        <v>0.88464</v>
       </c>
     </row>
     <row r="202">
@@ -2045,7 +2045,7 @@
         <v>200</v>
       </c>
       <c r="B202" t="n">
-        <v>0.85675</v>
+        <v>0.8719</v>
       </c>
     </row>
     <row r="203">
@@ -2053,7 +2053,7 @@
         <v>201</v>
       </c>
       <c r="B203" t="n">
-        <v>0.8512999999999999</v>
+        <v>0.88464</v>
       </c>
     </row>
     <row r="204">
@@ -2061,7 +2061,7 @@
         <v>202</v>
       </c>
       <c r="B204" t="n">
-        <v>0.84345</v>
+        <v>0.90523</v>
       </c>
     </row>
     <row r="205">
@@ -2069,7 +2069,7 @@
         <v>203</v>
       </c>
       <c r="B205" t="n">
-        <v>0.83799</v>
+        <v>0.89641</v>
       </c>
     </row>
     <row r="206">
@@ -2077,7 +2077,7 @@
         <v>204</v>
       </c>
       <c r="B206" t="n">
-        <v>0.91951</v>
+        <v>0.91046</v>
       </c>
     </row>
     <row r="207">
@@ -2085,7 +2085,7 @@
         <v>205</v>
       </c>
       <c r="B207" t="n">
-        <v>0.89802</v>
+        <v>0.92059</v>
       </c>
     </row>
     <row r="208">
@@ -2093,7 +2093,7 @@
         <v>206</v>
       </c>
       <c r="B208" t="n">
-        <v>0.88336</v>
+        <v>0.92843</v>
       </c>
     </row>
     <row r="209">
@@ -2101,7 +2101,7 @@
         <v>207</v>
       </c>
       <c r="B209" t="n">
-        <v>0.86869</v>
+        <v>0.93333</v>
       </c>
     </row>
     <row r="210">
@@ -2109,7 +2109,7 @@
         <v>208</v>
       </c>
       <c r="B210" t="n">
-        <v>0.86187</v>
+        <v>0.9359499999999999</v>
       </c>
     </row>
     <row r="211">
@@ -2117,7 +2117,7 @@
         <v>209</v>
       </c>
       <c r="B211" t="n">
-        <v>0.86733</v>
+        <v>0.9385599999999999</v>
       </c>
     </row>
     <row r="212">
@@ -2125,7 +2125,7 @@
         <v>210</v>
       </c>
       <c r="B212" t="n">
-        <v>0.87551</v>
+        <v>0.94346</v>
       </c>
     </row>
     <row r="213">
@@ -2133,7 +2133,7 @@
         <v>211</v>
       </c>
       <c r="B213" t="n">
-        <v>0.8819900000000001</v>
+        <v>0.94118</v>
       </c>
     </row>
     <row r="214">
@@ -2141,7 +2141,7 @@
         <v>212</v>
       </c>
       <c r="B214" t="n">
-        <v>0.8779</v>
+        <v>0.92582</v>
       </c>
     </row>
     <row r="215">
@@ -2149,7 +2149,7 @@
         <v>213</v>
       </c>
       <c r="B215" t="n">
-        <v>0.88063</v>
+        <v>0.9359499999999999</v>
       </c>
     </row>
     <row r="216">
@@ -2157,7 +2157,7 @@
         <v>214</v>
       </c>
       <c r="B216" t="n">
-        <v>0.8779</v>
+        <v>0.92582</v>
       </c>
     </row>
     <row r="217">
@@ -2165,7 +2165,7 @@
         <v>215</v>
       </c>
       <c r="B217" t="n">
-        <v>0.89018</v>
+        <v>0.9385599999999999</v>
       </c>
     </row>
     <row r="218">
@@ -2173,7 +2173,7 @@
         <v>216</v>
       </c>
       <c r="B218" t="n">
-        <v>0.90211</v>
+        <v>0.91797</v>
       </c>
     </row>
     <row r="219">
@@ -2181,7 +2181,7 @@
         <v>217</v>
       </c>
       <c r="B219" t="n">
-        <v>0.91405</v>
+        <v>0.91046</v>
       </c>
     </row>
     <row r="220">
@@ -2189,7 +2189,7 @@
         <v>218</v>
       </c>
       <c r="B220" t="n">
-        <v>0.90996</v>
+        <v>0.91797</v>
       </c>
     </row>
     <row r="221">
@@ -2197,7 +2197,7 @@
         <v>219</v>
       </c>
       <c r="B221" t="n">
-        <v>0.91542</v>
+        <v>0.8924800000000001</v>
       </c>
     </row>
     <row r="222">
@@ -2205,7 +2205,7 @@
         <v>220</v>
       </c>
       <c r="B222" t="n">
-        <v>0.92326</v>
+        <v>0.90915</v>
       </c>
     </row>
     <row r="223">
@@ -2213,7 +2213,7 @@
         <v>221</v>
       </c>
       <c r="B223" t="n">
-        <v>0.9222399999999999</v>
+        <v>0.8951</v>
       </c>
     </row>
     <row r="224">
@@ -2221,7 +2221,7 @@
         <v>222</v>
       </c>
       <c r="B224" t="n">
-        <v>0.91269</v>
+        <v>0.8924800000000001</v>
       </c>
     </row>
     <row r="225">
@@ -2229,7 +2229,7 @@
         <v>223</v>
       </c>
       <c r="B225" t="n">
-        <v>0.90757</v>
+        <v>0.89771</v>
       </c>
     </row>
     <row r="226">
@@ -2237,7 +2237,7 @@
         <v>224</v>
       </c>
       <c r="B226" t="n">
-        <v>0.90621</v>
+        <v>0.88725</v>
       </c>
     </row>
     <row r="227">
@@ -2245,7 +2245,7 @@
         <v>225</v>
       </c>
       <c r="B227" t="n">
-        <v>0.89393</v>
+        <v>0.87451</v>
       </c>
     </row>
     <row r="228">
@@ -2253,7 +2253,7 @@
         <v>226</v>
       </c>
       <c r="B228" t="n">
-        <v>0.88881</v>
+        <v>0.8924800000000001</v>
       </c>
     </row>
     <row r="229">
@@ -2261,7 +2261,7 @@
         <v>227</v>
       </c>
       <c r="B229" t="n">
-        <v>0.90484</v>
+        <v>0.8719</v>
       </c>
     </row>
     <row r="230">
@@ -2269,7 +2269,7 @@
         <v>228</v>
       </c>
       <c r="B230" t="n">
-        <v>0.91814</v>
+        <v>0.86699</v>
       </c>
     </row>
     <row r="231">
@@ -2277,7 +2277,7 @@
         <v>229</v>
       </c>
       <c r="B231" t="n">
-        <v>0.93827</v>
+        <v>0.86699</v>
       </c>
     </row>
     <row r="232">
@@ -2285,7 +2285,7 @@
         <v>230</v>
       </c>
       <c r="B232" t="n">
-        <v>0.93827</v>
+        <v>0.84902</v>
       </c>
     </row>
     <row r="233">
@@ -2293,7 +2293,7 @@
         <v>231</v>
       </c>
       <c r="B233" t="n">
-        <v>0.9502</v>
+        <v>0.85915</v>
       </c>
     </row>
     <row r="234">
@@ -2301,7 +2301,7 @@
         <v>232</v>
       </c>
       <c r="B234" t="n">
-        <v>0.9369</v>
+        <v>0.85163</v>
       </c>
     </row>
     <row r="235">
@@ -2309,7 +2309,7 @@
         <v>233</v>
       </c>
       <c r="B235" t="n">
-        <v>0.94202</v>
+        <v>0.85915</v>
       </c>
     </row>
     <row r="236">
@@ -2317,7 +2317,7 @@
         <v>234</v>
       </c>
       <c r="B236" t="n">
-        <v>0.94748</v>
+        <v>0.87712</v>
       </c>
     </row>
     <row r="237">
@@ -2325,7 +2325,7 @@
         <v>235</v>
       </c>
       <c r="B237" t="n">
-        <v>0.94202</v>
+        <v>0.89379</v>
       </c>
     </row>
     <row r="238">
@@ -2333,7 +2333,7 @@
         <v>236</v>
       </c>
       <c r="B238" t="n">
-        <v>0.9369</v>
+        <v>0.89771</v>
       </c>
     </row>
     <row r="239">
@@ -2341,7 +2341,7 @@
         <v>237</v>
       </c>
       <c r="B239" t="n">
-        <v>0.9341699999999999</v>
+        <v>0.93333</v>
       </c>
     </row>
     <row r="240">
@@ -2349,7 +2349,7 @@
         <v>238</v>
       </c>
       <c r="B240" t="n">
-        <v>0.9369</v>
+        <v>0.9219000000000001</v>
       </c>
     </row>
     <row r="241">
@@ -2357,7 +2357,7 @@
         <v>239</v>
       </c>
       <c r="B241" t="n">
-        <v>0.93145</v>
+        <v>0.88464</v>
       </c>
     </row>
     <row r="242">
@@ -2365,7 +2365,7 @@
         <v>240</v>
       </c>
       <c r="B242" t="n">
-        <v>0.93554</v>
+        <v>0.88464</v>
       </c>
     </row>
     <row r="243">
@@ -2373,7 +2373,7 @@
         <v>241</v>
       </c>
       <c r="B243" t="n">
-        <v>0.93827</v>
+        <v>0.86961</v>
       </c>
     </row>
     <row r="244">
@@ -2381,7 +2381,7 @@
         <v>242</v>
       </c>
       <c r="B244" t="n">
-        <v>0.92326</v>
+        <v>0.86961</v>
       </c>
     </row>
     <row r="245">
@@ -2389,7 +2389,7 @@
         <v>243</v>
       </c>
       <c r="B245" t="n">
-        <v>0.90996</v>
+        <v>0.86438</v>
       </c>
     </row>
     <row r="246">
@@ -2397,7 +2397,7 @@
         <v>244</v>
       </c>
       <c r="B246" t="n">
-        <v>0.92326</v>
+        <v>0.84641</v>
       </c>
     </row>
     <row r="247">
@@ -2405,7 +2405,7 @@
         <v>245</v>
       </c>
       <c r="B247" t="n">
-        <v>0.94475</v>
+        <v>0.82092</v>
       </c>
     </row>
     <row r="248">
@@ -2413,7 +2413,7 @@
         <v>246</v>
       </c>
       <c r="B248" t="n">
-        <v>0.93554</v>
+        <v>0.83627</v>
       </c>
     </row>
     <row r="249">
@@ -2421,7 +2421,7 @@
         <v>247</v>
       </c>
       <c r="B249" t="n">
-        <v>0.9502</v>
+        <v>0.77092</v>
       </c>
     </row>
     <row r="250">
@@ -2429,7 +2429,7 @@
         <v>248</v>
       </c>
       <c r="B250" t="n">
-        <v>0.96078</v>
+        <v>0.79281</v>
       </c>
     </row>
     <row r="251">
@@ -2437,7 +2437,103 @@
         <v>249</v>
       </c>
       <c r="B251" t="n">
-        <v>0.96896</v>
+        <v>0.78889</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" s="1" t="n">
+        <v>250</v>
+      </c>
+      <c r="B252" t="n">
+        <v>0.75686</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" s="1" t="n">
+        <v>251</v>
+      </c>
+      <c r="B253" t="n">
+        <v>0.75686</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" s="1" t="n">
+        <v>252</v>
+      </c>
+      <c r="B254" t="n">
+        <v>0.78137</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" s="1" t="n">
+        <v>253</v>
+      </c>
+      <c r="B255" t="n">
+        <v>0.78889</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" s="1" t="n">
+        <v>254</v>
+      </c>
+      <c r="B256" t="n">
+        <v>0.79542</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" s="1" t="n">
+        <v>255</v>
+      </c>
+      <c r="B257" t="n">
+        <v>0.82092</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" s="1" t="n">
+        <v>256</v>
+      </c>
+      <c r="B258" t="n">
+        <v>0.83366</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" s="1" t="n">
+        <v>257</v>
+      </c>
+      <c r="B259" t="n">
+        <v>0.83889</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" s="1" t="n">
+        <v>258</v>
+      </c>
+      <c r="B260" t="n">
+        <v>0.83235</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" s="1" t="n">
+        <v>259</v>
+      </c>
+      <c r="B261" t="n">
+        <v>0.82712</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" s="1" t="n">
+        <v>260</v>
+      </c>
+      <c r="B262" t="n">
+        <v>0.85654</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" s="1" t="n">
+        <v>261</v>
+      </c>
+      <c r="B263" t="n">
+        <v>0.85425</v>
       </c>
     </row>
   </sheetData>

</xml_diff>